<commit_message>
updated docs to view image plus raw excel
</commit_message>
<xml_diff>
--- a/docs/medicationadministration.xlsx
+++ b/docs/medicationadministration.xlsx
@@ -180,7 +180,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id
+    <t xml:space="preserve">id {[]} {[]}
 </t>
   </si>
   <si>
@@ -199,7 +199,7 @@
     <t>MedicationAdministration.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Meta
+    <t xml:space="preserve">Meta {[]} {[]}
 </t>
   </si>
   <si>
@@ -215,7 +215,7 @@
     <t>MedicationAdministration.implicitRules</t>
   </si>
   <si>
-    <t xml:space="preserve">uri
+    <t xml:space="preserve">uri {[]} {[]}
 </t>
   </si>
   <si>
@@ -235,7 +235,7 @@
     <t>MedicationAdministration.language</t>
   </si>
   <si>
-    <t xml:space="preserve">code
+    <t xml:space="preserve">code {[]} {[]}
 </t>
   </si>
   <si>
@@ -267,7 +267,7 @@
 htmlxhtmldisplay</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrative
+    <t xml:space="preserve">Narrative {[]} {[]}
 </t>
   </si>
   <si>
@@ -297,7 +297,7 @@
 anonymous resourcescontained resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource
+    <t xml:space="preserve">Resource {[]} {[]}
 </t>
   </si>
   <si>
@@ -323,7 +323,7 @@
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension
+    <t xml:space="preserve">Extension {[]} {[]}
 </t>
   </si>
   <si>
@@ -354,7 +354,7 @@
     <t>MedicationAdministration.identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifier
+    <t xml:space="preserve">Identifier {[]} {[]}
 </t>
   </si>
   <si>
@@ -376,8 +376,8 @@
     <t>MedicationAdministration.definition</t>
   </si>
   <si>
-    <t>Reference {http://hl7.org/fhir/StructureDefinition/PlanDefinition}
-Reference {http://hl7.org/fhir/StructureDefinition/ActivityDefinition}</t>
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/PlanDefinition], CanonicalType[http://hl7.org/fhir/StructureDefinition/ActivityDefinition]]}
+</t>
   </si>
   <si>
     <t>Instantiates protocol or definition</t>
@@ -395,8 +395,8 @@
     <t>MedicationAdministration.partOf</t>
   </si>
   <si>
-    <t>Reference {http://hl7.org/fhir/StructureDefinition/MedicationAdministration}
-Reference {http://hl7.org/fhir/StructureDefinition/Procedure}</t>
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/MedicationAdministration], CanonicalType[http://hl7.org/fhir/StructureDefinition/Procedure]]}
+</t>
   </si>
   <si>
     <t>Part of referenced event</t>
@@ -447,7 +447,7 @@
     <t>MedicationAdministration.category</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept
+    <t xml:space="preserve">CodeableConcept {[]} {[]}
 </t>
   </si>
   <si>
@@ -472,8 +472,8 @@
     <t>MedicationAdministration.medication[x]</t>
   </si>
   <si>
-    <t>CodeableConcept
-Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-medication}</t>
+    <t>CodeableConcept {[]} {[]}
+Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-medication]]}</t>
   </si>
   <si>
     <t>What was administered</t>
@@ -506,7 +506,7 @@
     <t>MedicationAdministration.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient]]}
 </t>
   </si>
   <si>
@@ -531,8 +531,8 @@
     <t>MedicationAdministration.context</t>
   </si>
   <si>
-    <t>Reference {http://hl7.org/fhir/StructureDefinition/Encounter}
-Reference {http://hl7.org/fhir/StructureDefinition/EpisodeOfCare}</t>
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Encounter], CanonicalType[http://hl7.org/fhir/StructureDefinition/EpisodeOfCare]]}
+</t>
   </si>
   <si>
     <t>Encounter or Episode of Care administered as part of</t>
@@ -556,7 +556,7 @@
     <t>MedicationAdministration.supportingInformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/Resource}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Resource]]}
 </t>
   </si>
   <si>
@@ -572,8 +572,8 @@
     <t>MedicationAdministration.effective[x]</t>
   </si>
   <si>
-    <t>dateTime
-Period</t>
+    <t>dateTime {[]} {[]}
+Period {[]} {[]}</t>
   </si>
   <si>
     <t>Start and end time of administration</t>
@@ -597,7 +597,7 @@
     <t>MedicationAdministration.performer</t>
   </si>
   <si>
-    <t xml:space="preserve">BackboneElement
+    <t xml:space="preserve">BackboneElement {[]} {[]}
 </t>
   </si>
   <si>
@@ -626,7 +626,7 @@
     <t>MedicationAdministration.performer.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string
+    <t xml:space="preserve">string {[]} {[]}
 </t>
   </si>
   <si>
@@ -667,8 +667,8 @@
     <t>MedicationAdministration.performer.actor</t>
   </si>
   <si>
-    <t>Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner}
-Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient}Reference {http://hl7.org/fhir/StructureDefinition/RelatedPerson}</t>
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner], CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson]]}
+</t>
   </si>
   <si>
     <t>Individual who was performing</t>
@@ -686,7 +686,7 @@
     <t>MedicationAdministration.performer.onBehalfOf</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/Organization}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization]]}
 </t>
   </si>
   <si>
@@ -705,7 +705,7 @@
     <t>MedicationAdministration.notGiven</t>
   </si>
   <si>
-    <t xml:space="preserve">boolean
+    <t xml:space="preserve">boolean {[]} {[]}
 </t>
   </si>
   <si>
@@ -792,8 +792,8 @@
     <t>MedicationAdministration.reasonReference</t>
   </si>
   <si>
-    <t>Reference {http://hl7.org/fhir/StructureDefinition/Condition}
-Reference {http://hl7.org/fhir/StructureDefinition/Observation}</t>
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Condition], CanonicalType[http://hl7.org/fhir/StructureDefinition/Observation]]}
+</t>
   </si>
   <si>
     <t>Condition or Observation that supports why the medication was administered</t>
@@ -820,7 +820,7 @@
     <t>MedicationAdministration.prescription</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/MedicationRequest}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/MedicationRequest]]}
 </t>
   </si>
   <si>
@@ -842,7 +842,7 @@
     <t>MedicationAdministration.device</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/Device}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Device]]}
 </t>
   </si>
   <si>
@@ -861,7 +861,7 @@
     <t>MedicationAdministration.note</t>
   </si>
   <si>
-    <t xml:space="preserve">Annotation
+    <t xml:space="preserve">Annotation {[]} {[]}
 </t>
   </si>
   <si>
@@ -988,7 +988,7 @@
     <t>MedicationAdministration.dosage.dose</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity {http://hl7.org/fhir/StructureDefinition/SimpleQuantity}
+    <t xml:space="preserve">Quantity {[CanonicalType[http://hl7.org/fhir/StructureDefinition/SimpleQuantity]]} {[]}
 </t>
   </si>
   <si>
@@ -1010,8 +1010,8 @@
     <t>MedicationAdministration.dosage.rate[x]</t>
   </si>
   <si>
-    <t>Ratio
-Quantity {http://hl7.org/fhir/StructureDefinition/SimpleQuantity}</t>
+    <t>Ratio {[]} {[]}
+Quantity {[CanonicalType[http://hl7.org/fhir/StructureDefinition/SimpleQuantity]]} {[]}</t>
   </si>
   <si>
     <t>Dose quantity per unit of time</t>
@@ -1032,7 +1032,7 @@
     <t>MedicationAdministration.eventHistory</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/Provenance}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Provenance]]}
 </t>
   </si>
   <si>

</xml_diff>